<commit_message>
sr: oncho update forms
</commit_message>
<xml_diff>
--- a/ONCHO/OEM/Sierra Leone/sr_oncho_oem_1_site_202211.xlsx
+++ b/ONCHO/OEM/Sierra Leone/sr_oncho_oem_1_site_202211.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="135">
   <si>
     <t>type</t>
   </si>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>list_name</t>
-  </si>
-  <si>
-    <t>label</t>
   </si>
   <si>
     <t>district_list</t>
@@ -1561,7 +1558,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -1894,7 +1891,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -1914,62 +1911,62 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="8" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" s="10" customFormat="1" spans="1:4">
       <c r="A2" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" s="10" customFormat="1" spans="1:4">
       <c r="A3" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="17"/>
     </row>
     <row r="4" s="10" customFormat="1" spans="1:4">
       <c r="A4" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" s="17"/>
     </row>
     <row r="5" s="10" customFormat="1" spans="1:4">
       <c r="A5" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D5" s="17"/>
     </row>
@@ -1981,25 +1978,25 @@
     </row>
     <row r="7" s="10" customFormat="1" spans="1:4">
       <c r="A7" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>71</v>
-      </c>
       <c r="C7" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D7" s="17"/>
     </row>
     <row r="8" s="10" customFormat="1" spans="1:4">
       <c r="A8" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D8" s="17"/>
     </row>
@@ -2011,73 +2008,73 @@
     </row>
     <row r="10" s="10" customFormat="1" spans="1:4">
       <c r="A10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="15" t="s">
-        <v>74</v>
-      </c>
       <c r="C10" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="17"/>
     </row>
     <row r="11" s="10" customFormat="1" spans="1:4">
       <c r="A11" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D11" s="17"/>
     </row>
     <row r="12" s="10" customFormat="1" spans="1:4">
       <c r="A12" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="17"/>
     </row>
     <row r="13" s="10" customFormat="1" spans="1:4">
       <c r="A13" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="17"/>
     </row>
     <row r="14" s="10" customFormat="1" spans="1:4">
       <c r="A14" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" s="17"/>
     </row>
     <row r="15" s="10" customFormat="1" spans="1:4">
       <c r="A15" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" s="17"/>
     </row>
@@ -2089,73 +2086,73 @@
     </row>
     <row r="17" s="10" customFormat="1" spans="1:4">
       <c r="A17" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="17"/>
     </row>
     <row r="18" s="10" customFormat="1" spans="1:4">
       <c r="A18" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D18" s="17"/>
     </row>
     <row r="19" s="10" customFormat="1" spans="1:4">
       <c r="A19" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="17"/>
     </row>
     <row r="20" s="10" customFormat="1" spans="1:4">
       <c r="A20" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" s="17"/>
     </row>
     <row r="21" s="10" customFormat="1" spans="1:4">
       <c r="A21" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D21" s="17"/>
     </row>
     <row r="22" s="10" customFormat="1" spans="1:4">
       <c r="A22" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" s="17"/>
     </row>
@@ -2167,227 +2164,227 @@
     </row>
     <row r="24" s="10" customFormat="1" spans="1:4">
       <c r="A24" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" s="17"/>
     </row>
     <row r="25" s="10" customFormat="1" spans="1:4">
       <c r="A25" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D25" s="17"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B42">
         <v>101</v>
@@ -2396,12 +2393,12 @@
         <v>101</v>
       </c>
       <c r="E42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B43">
         <v>102</v>
@@ -2410,12 +2407,12 @@
         <v>102</v>
       </c>
       <c r="E43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B44">
         <v>103</v>
@@ -2424,12 +2421,12 @@
         <v>103</v>
       </c>
       <c r="E44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B45">
         <v>104</v>
@@ -2438,12 +2435,12 @@
         <v>104</v>
       </c>
       <c r="E45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B46">
         <v>105</v>
@@ -2452,12 +2449,12 @@
         <v>105</v>
       </c>
       <c r="E46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B47">
         <v>106</v>
@@ -2466,12 +2463,12 @@
         <v>106</v>
       </c>
       <c r="E47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B48">
         <v>107</v>
@@ -2480,12 +2477,12 @@
         <v>107</v>
       </c>
       <c r="E48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B49">
         <v>108</v>
@@ -2494,12 +2491,12 @@
         <v>108</v>
       </c>
       <c r="E49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B50">
         <v>109</v>
@@ -2508,12 +2505,12 @@
         <v>109</v>
       </c>
       <c r="E50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B51">
         <v>110</v>
@@ -2522,12 +2519,12 @@
         <v>110</v>
       </c>
       <c r="E51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52">
         <v>111</v>
@@ -2536,12 +2533,12 @@
         <v>111</v>
       </c>
       <c r="E52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B53">
         <v>112</v>
@@ -2550,175 +2547,175 @@
         <v>112</v>
       </c>
       <c r="E53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55">
         <v>101</v>
       </c>
       <c r="C55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D55" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56">
         <v>102</v>
       </c>
       <c r="C56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B57">
         <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B58">
         <v>104</v>
       </c>
       <c r="C58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D58" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B59">
         <v>105</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D59" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B60">
         <v>106</v>
       </c>
       <c r="C60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B61">
         <v>107</v>
       </c>
       <c r="C61" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B62">
         <v>108</v>
       </c>
       <c r="C62" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B63">
         <v>109</v>
       </c>
       <c r="C63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B64">
         <v>110</v>
       </c>
       <c r="C64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B65">
         <v>111</v>
       </c>
       <c r="C65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D65" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B66">
         <v>112</v>
       </c>
       <c r="C66" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D66" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2736,7 +2733,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -2748,27 +2745,27 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
         <v>119</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>120</v>
-      </c>
-      <c r="C2" t="s">
-        <v>121</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2803,28 +2800,28 @@
   <sheetData>
     <row r="1" ht="26.25" spans="1:10">
       <c r="A1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>126</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" ht="26.25" spans="1:10">
@@ -2832,25 +2829,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2">
         <v>101</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" ht="26.25" spans="1:10">
@@ -2858,25 +2855,25 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="E3">
         <v>102</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" ht="26.25" spans="1:10">
@@ -2884,23 +2881,23 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4">
         <v>103</v>
       </c>
       <c r="G4"/>
       <c r="I4" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" ht="26.25" spans="1:10">
@@ -2908,23 +2905,23 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5">
         <v>104</v>
       </c>
       <c r="G5"/>
       <c r="I5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" ht="26.25" spans="1:10">
@@ -2932,23 +2929,23 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6">
         <v>105</v>
       </c>
       <c r="G6"/>
       <c r="I6" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" ht="26.25" spans="1:10">
@@ -2956,23 +2953,23 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E7">
         <v>106</v>
       </c>
       <c r="G7"/>
       <c r="I7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" ht="26.25" spans="1:10">
@@ -2980,23 +2977,23 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8">
         <v>107</v>
       </c>
       <c r="G8"/>
       <c r="I8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" ht="26.25" spans="1:10">
@@ -3004,21 +3001,21 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9">
         <v>108</v>
       </c>
       <c r="G9"/>
       <c r="I9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" ht="26.25" spans="1:10">
@@ -3026,23 +3023,23 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E10">
         <v>109</v>
       </c>
       <c r="G10"/>
       <c r="I10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" ht="26.25" spans="1:10">
@@ -3050,21 +3047,21 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11">
         <v>110</v>
       </c>
       <c r="G11"/>
       <c r="I11" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" ht="26.25" spans="1:10">
@@ -3072,21 +3069,21 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E12">
         <v>111</v>
       </c>
       <c r="G12"/>
       <c r="I12" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" ht="26.25" spans="1:10">
@@ -3094,23 +3091,23 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E13">
         <v>112</v>
       </c>
       <c r="G13"/>
       <c r="I13" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sr: update site form
</commit_message>
<xml_diff>
--- a/ONCHO/OEM/Sierra Leone/sr_oncho_oem_1_site_202211.xlsx
+++ b/ONCHO/OEM/Sierra Leone/sr_oncho_oem_1_site_202211.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="130">
   <si>
     <t>type</t>
   </si>
@@ -1553,7 +1553,7 @@
   <sheetPr/>
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -1851,12 +1851,12 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A52" sqref="$A52:$XFD56"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="$A76:$XFD76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="4"/>
@@ -2742,6 +2742,96 @@
       <c r="D69"/>
       <c r="E69" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>108</v>
+      </c>
+      <c r="B70">
+        <v>119</v>
+      </c>
+      <c r="C70">
+        <v>119</v>
+      </c>
+      <c r="D70"/>
+      <c r="E70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71">
+        <v>120</v>
+      </c>
+      <c r="C71">
+        <v>120</v>
+      </c>
+      <c r="D71"/>
+      <c r="E71" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>108</v>
+      </c>
+      <c r="B72">
+        <v>121</v>
+      </c>
+      <c r="C72">
+        <v>121</v>
+      </c>
+      <c r="D72"/>
+      <c r="E72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>108</v>
+      </c>
+      <c r="B73">
+        <v>122</v>
+      </c>
+      <c r="C73">
+        <v>122</v>
+      </c>
+      <c r="D73"/>
+      <c r="E73" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>108</v>
+      </c>
+      <c r="B74">
+        <v>123</v>
+      </c>
+      <c r="C74">
+        <v>123</v>
+      </c>
+      <c r="D74"/>
+      <c r="E74" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>108</v>
+      </c>
+      <c r="B75">
+        <v>124</v>
+      </c>
+      <c r="C75">
+        <v>124</v>
+      </c>
+      <c r="D75"/>
+      <c r="E75" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>